<commit_message>
excel file and Base test class is done
</commit_message>
<xml_diff>
--- a/data/input.xlsx
+++ b/data/input.xlsx
@@ -1,24 +1,53 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="12180" windowHeight="6420"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="ValidLogin" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="125725"/>
+  <oleSize ref="A1"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>HomePageTitle</t>
+  </si>
+  <si>
+    <t>purnendukumar82</t>
+  </si>
+  <si>
+    <t>actiTIME-Enter Time-Track</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -46,8 +75,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -342,13 +372,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>8706</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Test Classes are updated
</commit_message>
<xml_diff>
--- a/data/input.xlsx
+++ b/data/input.xlsx
@@ -4,20 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="12180" windowHeight="6420"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="12180" windowHeight="6420" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ValidLogin" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="InvalidLogin" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <oleSize ref="A1"/>
+  <oleSize ref="A1:L20"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>UserName</t>
   </si>
@@ -32,13 +32,22 @@
   </si>
   <si>
     <t>actiTIME-Enter Time-Track</t>
+  </si>
+  <si>
+    <t>Error message</t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>Username or Password is invalid. Please try again.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -53,6 +62,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCE0100"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -75,9 +90,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -374,8 +390,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -413,13 +429,51 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="44.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>111</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="C4" s="2"/>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="C5" s="2"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>